<commit_message>
editting examples in get-dat.R
</commit_message>
<xml_diff>
--- a/inst/extdata/maturity_codes.xlsx
+++ b/inst/extdata/maturity_codes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="144" windowWidth="30660" windowHeight="14280" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="144" windowWidth="30660" windowHeight="14280"/>
   </bookViews>
   <sheets>
     <sheet name="mat convens, codes and descrips" sheetId="1" r:id="rId1"/>
@@ -1197,12 +1197,6 @@
     <t xml:space="preserve">                  (COUNT(SP.SPECIMEN_SEX_CODE) &lt;&gt; 0) AND (NOT (SUM(SM.CATCH_COUNT) IS NULL))</t>
   </si>
   <si>
-    <t>dana - maturity for females at 3, males at 2/3? Convention not used?</t>
-  </si>
-  <si>
-    <t>confirm with Jackie</t>
-  </si>
-  <si>
     <t>SELECT MC.MATURITY_CONVENTION_CODE AS MAT_CONV_CODE, MC.MATURITY_CONVENTION_DESC AS MAT_CONV_DESC, MD.SPECIMEN_SEX_CODE, MC.MATURITY_CONVENTION_MAXVALUE,</t>
   </si>
   <si>
@@ -1234,6 +1228,12 @@
   </si>
   <si>
     <t>mature_at</t>
+  </si>
+  <si>
+    <t>confirmed against Jackie's code sheets</t>
+  </si>
+  <si>
+    <t>dana - 3 for both genders</t>
   </si>
 </sst>
 </file>
@@ -1602,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I344"/>
   <sheetViews>
-    <sheetView topLeftCell="A274" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40:D43"/>
+    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
+      <selection activeCell="D347" sqref="D347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10705,7 +10705,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10957,13 +10957,13 @@
         <v>2017</v>
       </c>
       <c r="F12" s="3">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>384</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -10989,7 +10989,7 @@
         <v>385</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -11052,7 +11052,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>392</v>
+        <v>404</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -11141,7 +11141,7 @@
         <v>385</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -11152,13 +11152,13 @@
         <v>224</v>
       </c>
       <c r="F21" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>384</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -11338,10 +11338,10 @@
         <v>2011</v>
       </c>
       <c r="F30" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>393</v>
+        <v>403</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
@@ -11619,27 +11619,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E49"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>398</v>
+      </c>
+      <c r="B1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" t="s">
         <v>400</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>401</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>402</v>
-      </c>
-      <c r="D1" t="s">
-        <v>403</v>
-      </c>
-      <c r="E1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -11945,7 +11945,7 @@
         <v>99</v>
       </c>
       <c r="E19">
-        <v>55</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -12467,7 +12467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -12475,7 +12475,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -12490,7 +12490,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -12500,17 +12500,17 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -12525,7 +12525,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>